<commit_message>
Update December 2020 - Reformat grillage wizard into 'Analysis.py' - Add unit test for Analysis.py (Analysis_test.py)
</commit_message>
<xml_diff>
--- a/Bridge model opensees/Benchmark bridge.xlsx
+++ b/Bridge model opensees/Benchmark bridge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicni\PycharmProjects\Opensees-project\Bridge model opensees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7E68A3-F7D4-4F40-A021-4E6974F7D04C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C378185F-03FB-40C2-8A09-9A6FEBB4D7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1296" yWindow="3780" windowWidth="8556" windowHeight="7224" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node" sheetId="1" r:id="rId1"/>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="L19" sqref="L18:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2723,8 +2723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H22:H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5070,7 +5070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update 4/2/2021 - Alpha stage sphinx documentation - Unit test works
</commit_message>
<xml_diff>
--- a/Bridge model opensees/Benchmark bridge.xlsx
+++ b/Bridge model opensees/Benchmark bridge.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicni\PycharmProjects\Opensees-project\Bridge model opensees\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicni\PycharmProjects\Opensees-project2\Bridge model opensees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C378185F-03FB-40C2-8A09-9A6FEBB4D7EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5429E0C-8EF8-4756-8A9E-60F89ABCF22F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node" sheetId="1" r:id="rId1"/>
     <sheet name="Connectivity" sheetId="2" r:id="rId2"/>
     <sheet name="Member" sheetId="3" r:id="rId3"/>
+    <sheet name="Member transformation" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="50">
   <si>
     <t>x</t>
   </si>
@@ -159,6 +160,30 @@
   </si>
   <si>
     <t>A(m^2)</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>trans</t>
+  </si>
+  <si>
+    <t>Trans tag</t>
+  </si>
+  <si>
+    <t>Name of variable saved in grillage class</t>
+  </si>
+  <si>
+    <t>Vector</t>
+  </si>
+  <si>
+    <t>[0,0,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transform tag </t>
   </si>
 </sst>
 </file>
@@ -2723,8 +2748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5068,31 +5093,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.109375" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.109375" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -5100,58 +5126,61 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>27</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -5159,31 +5188,34 @@
         <v>37</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>0.89600000000000002</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>34652200000</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>20000000000</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.13300000000000001</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.21299999999999999</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.25900000000000001</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.23300000000000001</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -5191,31 +5223,34 @@
         <v>38</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>0.89600000000000002</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>34652200000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>20000000000</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.13300000000000001</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.21299999999999999</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.25900000000000001</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.23300000000000001</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5223,31 +5258,34 @@
         <v>39</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>4.4624999999999998E-2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>34652200000</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>20000000000</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>2.5999999999999998E-4</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>1.1E-4</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>2.42E-4</v>
-      </c>
-      <c r="I4" s="2">
-        <v>3.7187499999999998E-2</v>
       </c>
       <c r="J4" s="2">
         <v>3.7187499999999998E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="K4" s="2">
+        <v>3.7187499999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -5255,67 +5293,126 @@
         <v>36</v>
       </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>0.44280000000000003</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>34652200000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>20000000000</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>2.2799999999999999E-3</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>0.2233</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <v>1.19556E-3</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.36899999999999999</v>
       </c>
       <c r="J5" s="2">
         <v>0.36899999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="K5" s="2">
+        <v>0.36899999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
         <v>0.22140000000000001</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>34652200000</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>20000000000</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>0.111</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>5.9699999999999998E-4</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.1845</v>
       </c>
       <c r="J6" s="2">
         <v>0.1845</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="C8" s="1"/>
+      <c r="K6" s="2">
+        <v>0.1845</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A3B36D-C2CF-4C3F-A9A4-C292E438CD8E}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update 10/2/2021 - Added doc to vcs
</commit_message>
<xml_diff>
--- a/Bridge model opensees/Benchmark bridge.xlsx
+++ b/Bridge model opensees/Benchmark bridge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicni\PycharmProjects\Opensees-project2\Bridge model opensees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5429E0C-8EF8-4756-8A9E-60F89ABCF22F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71CE57B-B247-4298-90BE-3213F81CAD04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11448" yWindow="1308" windowWidth="13020" windowHeight="10032" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="53">
   <si>
     <t>x</t>
   </si>
@@ -183,7 +183,16 @@
     <t>[1,0,0]</t>
   </si>
   <si>
-    <t xml:space="preserve">Transform tag </t>
+    <t>fixity code</t>
+  </si>
+  <si>
+    <t>RRRFFF</t>
+  </si>
+  <si>
+    <t>FRRFFF</t>
+  </si>
+  <si>
+    <t>Transform tag</t>
   </si>
 </sst>
 </file>
@@ -1034,15 +1043,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L18:L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1061,8 +1070,11 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1082,8 +1094,11 @@
       <c r="F2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>12</v>
       </c>
@@ -1102,8 +1117,11 @@
       <c r="F3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>23</v>
       </c>
@@ -1122,8 +1140,11 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>34</v>
       </c>
@@ -1142,8 +1163,11 @@
       <c r="F5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>45</v>
       </c>
@@ -1162,8 +1186,11 @@
       <c r="F6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>56</v>
       </c>
@@ -1182,8 +1209,11 @@
       <c r="F7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>67</v>
       </c>
@@ -1203,8 +1233,11 @@
       <c r="F8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <f>A2+1</f>
         <v>2</v>
@@ -1225,8 +1258,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <f t="shared" ref="A10:A73" si="1">A3+1</f>
         <v>13</v>
@@ -1247,8 +1283,11 @@
       <c r="F10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -1269,8 +1308,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -1291,8 +1333,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -1313,8 +1358,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -1335,8 +1383,11 @@
       <c r="F14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -1357,8 +1408,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>3</v>
@@ -1379,8 +1433,11 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -1401,8 +1458,11 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -1423,8 +1483,11 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -1445,8 +1508,11 @@
       <c r="F19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -1467,8 +1533,11 @@
       <c r="F20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -1489,8 +1558,11 @@
       <c r="F21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -1511,8 +1583,11 @@
       <c r="F22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -1533,8 +1608,11 @@
       <c r="F23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1555,8 +1633,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -1577,8 +1658,11 @@
       <c r="F25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -1599,8 +1683,11 @@
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -1621,8 +1708,11 @@
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -1643,8 +1733,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -1665,8 +1758,11 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -1687,8 +1783,11 @@
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -1709,8 +1808,11 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -1731,8 +1833,11 @@
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -1753,8 +1858,11 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -1775,8 +1883,11 @@
       <c r="F34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -1797,8 +1908,11 @@
       <c r="F35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -1819,8 +1933,11 @@
       <c r="F36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -1841,8 +1958,11 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -1863,8 +1983,11 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -1885,8 +2008,11 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -1907,8 +2033,11 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -1929,8 +2058,11 @@
       <c r="F41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -1951,8 +2083,11 @@
       <c r="F42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -1973,8 +2108,11 @@
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -1995,8 +2133,11 @@
       <c r="F44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -2017,8 +2158,11 @@
       <c r="F45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -2039,8 +2183,11 @@
       <c r="F46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -2061,8 +2208,11 @@
       <c r="F47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -2083,8 +2233,11 @@
       <c r="F48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -2105,8 +2258,11 @@
       <c r="F49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -2127,8 +2283,11 @@
       <c r="F50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -2149,8 +2308,11 @@
       <c r="F51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -2171,8 +2333,11 @@
       <c r="F52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -2193,8 +2358,11 @@
       <c r="F53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -2215,8 +2383,11 @@
       <c r="F54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -2237,8 +2408,11 @@
       <c r="F55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -2259,8 +2433,11 @@
       <c r="F56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -2281,8 +2458,11 @@
       <c r="F57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -2303,8 +2483,11 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -2325,8 +2508,11 @@
       <c r="F59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -2347,8 +2533,11 @@
       <c r="F60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -2369,8 +2558,11 @@
       <c r="F61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -2391,8 +2583,11 @@
       <c r="F62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -2413,8 +2608,11 @@
       <c r="F63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -2435,8 +2633,11 @@
       <c r="F64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -2457,8 +2658,11 @@
       <c r="F65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -2479,8 +2683,11 @@
       <c r="F66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:6">
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -2501,8 +2708,11 @@
       <c r="F67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -2523,8 +2733,11 @@
       <c r="F68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -2545,8 +2758,11 @@
       <c r="F69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -2567,8 +2783,11 @@
       <c r="F70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:6">
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -2589,8 +2808,11 @@
       <c r="F71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -2611,8 +2833,11 @@
       <c r="F72" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="G72" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -2632,8 +2857,11 @@
       <c r="F73" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="G73" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74">
         <f t="shared" ref="A74:A78" si="4">A67+1</f>
         <v>33</v>
@@ -2653,8 +2881,11 @@
       <c r="F74" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="75" spans="1:6">
+      <c r="G74" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75">
         <f t="shared" si="4"/>
         <v>44</v>
@@ -2674,8 +2905,11 @@
       <c r="F75" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="76" spans="1:6">
+      <c r="G75" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76">
         <f t="shared" si="4"/>
         <v>55</v>
@@ -2695,8 +2929,11 @@
       <c r="F76" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="G76" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77">
         <f t="shared" si="4"/>
         <v>66</v>
@@ -2716,8 +2953,11 @@
       <c r="F77" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="78" spans="1:6">
+      <c r="G77" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78">
         <f t="shared" si="4"/>
         <v>77</v>
@@ -2737,6 +2977,9 @@
       </c>
       <c r="F78" t="s">
         <v>17</v>
+      </c>
+      <c r="G78" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -5096,7 +5339,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5368,8 +5611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9A3B36D-C2CF-4C3F-A9A4-C292E438CD8E}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5381,7 +5624,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Node and mesh feature improvements - add function to calculate vector xz for geo trans of Opensees - redefined section for grillage member with ortho mesh 1 - long 2 - long edge beam 3 - trans region A 4 - trans between region A and B 5 - trans region B 6 - skewed members
</commit_message>
<xml_diff>
--- a/Bridge model opensees/Benchmark bridge.xlsx
+++ b/Bridge model opensees/Benchmark bridge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicni\PycharmProjects\Opensees-project2\Bridge model opensees\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C71CE57B-B247-4298-90BE-3213F81CAD04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3994B315-C801-4193-A12D-8C27A5496908}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11448" yWindow="1308" windowWidth="13020" windowHeight="10032" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7404" yWindow="1488" windowWidth="13020" windowHeight="10032" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Node" sheetId="1" r:id="rId1"/>
@@ -1046,7 +1046,7 @@
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>